<commit_message>
added code for new deal page
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testData/HubSpot_TestData.xlsx
+++ b/src/main/java/com/qa/testData/HubSpot_TestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramesh/eclipse-workspace/POMFramework/src/main/java/com/qa/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BA2236-B3D1-C44E-B9F5-94525C6E320C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679A8065-AC52-7A42-BFB1-82999FAA587E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" xr2:uid="{23B73170-BD47-474F-A13C-6197046ADD0B}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" activeTab="1" xr2:uid="{23B73170-BD47-474F-A13C-6197046ADD0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
+    <sheet name="Deals" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Email</t>
   </si>
@@ -36,25 +37,49 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>Hero</t>
-  </si>
-  <si>
-    <t>razzz</t>
-  </si>
-  <si>
-    <t>LifeCycleStage</t>
+    <t>StageName</t>
+  </si>
+  <si>
+    <t>LeadStatus</t>
+  </si>
+  <si>
+    <t>New</t>
   </si>
   <si>
     <t>Lead</t>
   </si>
   <si>
-    <t>test@123g.com</t>
+    <t>Razz</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>ab2@abc.com</t>
+  </si>
+  <si>
+    <t>DealName</t>
+  </si>
+  <si>
+    <t>DealAmount</t>
+  </si>
+  <si>
+    <t>DealMonth</t>
+  </si>
+  <si>
+    <t>DealDay</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mmmm\ yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -93,9 +118,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -411,15 +437,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF3B25D-178D-9640-9413-57B510B1AAC8}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,21 +456,27 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -453,4 +485,50 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463F4429-E5CA-2741-B8D2-2D9D834C43AD}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="2">
+        <v>43983</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added code for new task
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/testData/HubSpot_TestData.xlsx
+++ b/src/main/java/com/qa/testData/HubSpot_TestData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ramesh/eclipse-workspace/POMFramework/src/main/java/com/qa/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679A8065-AC52-7A42-BFB1-82999FAA587E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB58D94-4826-CC4A-BE9C-43A4774DA41E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16620" activeTab="1" xr2:uid="{23B73170-BD47-474F-A13C-6197046ADD0B}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" activeTab="2" xr2:uid="{23B73170-BD47-474F-A13C-6197046ADD0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
     <sheet name="Deals" sheetId="2" r:id="rId2"/>
+    <sheet name="Tasks" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Email</t>
   </si>
@@ -43,43 +44,91 @@
     <t>LeadStatus</t>
   </si>
   <si>
+    <t>DealName</t>
+  </si>
+  <si>
+    <t>DealAmount</t>
+  </si>
+  <si>
+    <t>DealStage</t>
+  </si>
+  <si>
+    <t>Subscriber</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>JobTitle</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>DealType</t>
+  </si>
+  <si>
+    <t>DealCompany</t>
+  </si>
+  <si>
+    <t>DealConatct</t>
+  </si>
+  <si>
+    <t>New Business</t>
+  </si>
+  <si>
+    <t>Closed won</t>
+  </si>
+  <si>
+    <t>ffd9g.com</t>
+  </si>
+  <si>
+    <t>Raj Khanna (abcd1@abc.com)</t>
+  </si>
+  <si>
     <t>New</t>
   </si>
   <si>
-    <t>Lead</t>
-  </si>
-  <si>
-    <t>Razz</t>
-  </si>
-  <si>
-    <t>Ram</t>
-  </si>
-  <si>
-    <t>ab2@abc.com</t>
-  </si>
-  <si>
-    <t>DealName</t>
-  </si>
-  <si>
-    <t>DealAmount</t>
-  </si>
-  <si>
-    <t>DealMonth</t>
-  </si>
-  <si>
-    <t>DealDay</t>
-  </si>
-  <si>
-    <t>Test</t>
+    <t>Four</t>
+  </si>
+  <si>
+    <t>newfour@abc.com</t>
+  </si>
+  <si>
+    <t>NewFour</t>
+  </si>
+  <si>
+    <t>TaskTitle</t>
+  </si>
+  <si>
+    <t>TaskType</t>
+  </si>
+  <si>
+    <t>TaskDateValue</t>
+  </si>
+  <si>
+    <t>TaskTimeValue</t>
+  </si>
+  <si>
+    <t>Customdate</t>
+  </si>
+  <si>
+    <t>TaskAssociateWith</t>
+  </si>
+  <si>
+    <t>TaskQueueValue</t>
+  </si>
+  <si>
+    <t>Twelve</t>
+  </si>
+  <si>
+    <t>Tesy2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mmmm\ yyyy"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -121,7 +170,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -437,15 +486,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF3B25D-178D-9640-9413-57B510B1AAC8}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,22 +513,34 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="F2">
+        <v>1234567890</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -489,43 +553,120 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463F4429-E5CA-2741-B8D2-2D9D834C43AD}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>2000</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC62798E-DCC5-3749-A667-B5ADFCC7694F}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2">
-        <v>43983</v>
-      </c>
-      <c r="C2">
-        <v>25</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.45833333333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>